<commit_message>
[Silverfox] 가데이터 CSV 재수정
</commit_message>
<xml_diff>
--- a/DesignDocs/VariableData/Gimmick.xlsx
+++ b/DesignDocs/VariableData/Gimmick.xlsx
@@ -5,16 +5,16 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Silverfox_x\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\2D-Side-View-Roguelike\DesignDocs\VariableData\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{51812B90-CD34-47FE-AC86-40B309EF4D36}" xr6:coauthVersionLast="28" xr6:coauthVersionMax="28" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6044EDC6-807E-4123-8E7D-4E4BF3DB6006}" xr6:coauthVersionLast="28" xr6:coauthVersionMax="28" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="11175" xr2:uid="{46E70EC2-47F6-4A12-9747-1FCBE8C7A962}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="11175" activeTab="1" xr2:uid="{46E70EC2-47F6-4A12-9747-1FCBE8C7A962}"/>
   </bookViews>
   <sheets>
-    <sheet name="디스크립션" sheetId="2" r:id="rId1"/>
-    <sheet name="Gimmick" sheetId="1" r:id="rId2"/>
+    <sheet name="Gimmick" sheetId="1" r:id="rId1"/>
+    <sheet name="디스크립션" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="171027"/>
   <extLst>
@@ -495,6 +495,83 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F00B2F32-B102-4927-9519-834CA56DC18E}">
+  <dimension ref="A1:D4"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C15" sqref="C15"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="3" max="3" width="12.125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="13" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A2">
+        <v>1000</v>
+      </c>
+      <c r="B2" t="s">
+        <v>4</v>
+      </c>
+      <c r="C2" t="s">
+        <v>5</v>
+      </c>
+      <c r="D2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A3">
+        <v>2000</v>
+      </c>
+      <c r="B3" t="s">
+        <v>6</v>
+      </c>
+      <c r="C3" t="s">
+        <v>7</v>
+      </c>
+      <c r="D3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A4">
+        <v>2001</v>
+      </c>
+      <c r="B4" t="s">
+        <v>8</v>
+      </c>
+      <c r="C4" t="s">
+        <v>9</v>
+      </c>
+      <c r="D4">
+        <v>1</v>
+      </c>
+    </row>
+  </sheetData>
+  <phoneticPr fontId="1" type="noConversion"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1F9FFF29-637B-4E57-A6ED-96F05AAD7C31}">
   <dimension ref="B2:E13"/>
   <sheetViews>
@@ -622,81 +699,4 @@
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
-</file>
-
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F00B2F32-B102-4927-9519-834CA56DC18E}">
-  <dimension ref="A1:D4"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C15" sqref="C15"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
-  <cols>
-    <col min="3" max="3" width="12.125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="13" bestFit="1" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" t="s">
-        <v>1</v>
-      </c>
-      <c r="C1" t="s">
-        <v>2</v>
-      </c>
-      <c r="D1" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A2">
-        <v>1000</v>
-      </c>
-      <c r="B2" t="s">
-        <v>4</v>
-      </c>
-      <c r="C2" t="s">
-        <v>5</v>
-      </c>
-      <c r="D2">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A3">
-        <v>2000</v>
-      </c>
-      <c r="B3" t="s">
-        <v>6</v>
-      </c>
-      <c r="C3" t="s">
-        <v>7</v>
-      </c>
-      <c r="D3">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A4">
-        <v>2001</v>
-      </c>
-      <c r="B4" t="s">
-        <v>8</v>
-      </c>
-      <c r="C4" t="s">
-        <v>9</v>
-      </c>
-      <c r="D4">
-        <v>1</v>
-      </c>
-    </row>
-  </sheetData>
-  <phoneticPr fontId="1" type="noConversion"/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
-</worksheet>
 </file>
</xml_diff>